<commit_message>
updating data with NTP molecules in cluded
Pushing the TEST, and VEGA predictions, the cluster data, and the mutagenicity_data files as well as the selected descriptors files
</commit_message>
<xml_diff>
--- a/Final_Data/TEST_predictions.xlsx
+++ b/Final_Data/TEST_predictions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ResearchWorkingDirectory\Environmental_PAH_Mutagenicity\Final_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B0089C-9202-4A09-A712-31119D6B52BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E84F10B-A4EF-4183-A15C-4989E373CD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="1671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1797" uniqueCount="1797">
   <si>
     <t>Pred_Consensus</t>
   </si>
@@ -5033,6 +5033,384 @@
   </si>
   <si>
     <t>result_from_database</t>
+  </si>
+  <si>
+    <t>CC(COc1ccccc1)OCCCO</t>
+  </si>
+  <si>
+    <t>51730-94-0</t>
+  </si>
+  <si>
+    <t>Dipropylene glycol phenyl ether</t>
+  </si>
+  <si>
+    <t>Cc1ccccc1C(=O)O</t>
+  </si>
+  <si>
+    <t>118-90-1</t>
+  </si>
+  <si>
+    <t>o-Toluic acid</t>
+  </si>
+  <si>
+    <t>Cc1cccc(C)c1O</t>
+  </si>
+  <si>
+    <t>576-26-1</t>
+  </si>
+  <si>
+    <t>2,6-Dimethyl phenol</t>
+  </si>
+  <si>
+    <t>Cc1ccc2c(C)cccc2c1</t>
+  </si>
+  <si>
+    <t>575-43-9</t>
+  </si>
+  <si>
+    <t>1,6-Dimethylnaphthalene</t>
+  </si>
+  <si>
+    <t>CC(C)CCOC(=O)/C=C/c1ccccc1</t>
+  </si>
+  <si>
+    <t>7779-65-9</t>
+  </si>
+  <si>
+    <t>Isoamyl cinnamate</t>
+  </si>
+  <si>
+    <t>Cc1ccc(C(=O)O)cc1</t>
+  </si>
+  <si>
+    <t>99-94-5</t>
+  </si>
+  <si>
+    <t>p-Toluic acid</t>
+  </si>
+  <si>
+    <t>OCC1OC(Oc2ccc(O)cc2)C(O)C(O)C1O</t>
+  </si>
+  <si>
+    <t>497-76-7</t>
+  </si>
+  <si>
+    <t>Arbutin</t>
+  </si>
+  <si>
+    <t>Cc1ccccc1O</t>
+  </si>
+  <si>
+    <t>95-48-7</t>
+  </si>
+  <si>
+    <t>o-Cresol</t>
+  </si>
+  <si>
+    <t>CC(C)c1ccccc1</t>
+  </si>
+  <si>
+    <t>98-82-8</t>
+  </si>
+  <si>
+    <t>Cumene</t>
+  </si>
+  <si>
+    <t>Cc1ccc(C(C)(C)O)cc1</t>
+  </si>
+  <si>
+    <t>1197-01-9</t>
+  </si>
+  <si>
+    <t>p-Cymen-8-ol</t>
+  </si>
+  <si>
+    <t>Cc1ccc2ccccc2c1C</t>
+  </si>
+  <si>
+    <t>28804-88-8</t>
+  </si>
+  <si>
+    <t>Dimethylnaphthalene</t>
+  </si>
+  <si>
+    <t>O=C(O)c1ccc(O)cc1O</t>
+  </si>
+  <si>
+    <t>89-86-1</t>
+  </si>
+  <si>
+    <t>2,4-Dihydroxybenzoic acid</t>
+  </si>
+  <si>
+    <t>COc1cc(C2Oc3cc(C4Oc5cc(O)cc(O)c5C(=O)C4O)ccc3OC2CO)ccc1O</t>
+  </si>
+  <si>
+    <t>22888-70-6</t>
+  </si>
+  <si>
+    <t>Silybin</t>
+  </si>
+  <si>
+    <t>O=C(Cc1ccccc1)OCc1ccccc1</t>
+  </si>
+  <si>
+    <t>102-16-9</t>
+  </si>
+  <si>
+    <t>Benzyl phenylacetate</t>
+  </si>
+  <si>
+    <t>COCCOC(=O)c1ccccc1C(=O)OCCOC</t>
+  </si>
+  <si>
+    <t>117-82-8</t>
+  </si>
+  <si>
+    <t>Di(2-methoxyethyl)phthalate</t>
+  </si>
+  <si>
+    <t>CC(=O)c1cc(C)oc1C</t>
+  </si>
+  <si>
+    <t>10599-70-9</t>
+  </si>
+  <si>
+    <t>3-Acetyl-2,5-dimethylfuran</t>
+  </si>
+  <si>
+    <t>Cc1cc(C)cc(O)c1</t>
+  </si>
+  <si>
+    <t>108-68-9</t>
+  </si>
+  <si>
+    <t>3,5-Dimethyl phenol</t>
+  </si>
+  <si>
+    <t>Cc1ccc(O)c(O)c1</t>
+  </si>
+  <si>
+    <t>452-86-8</t>
+  </si>
+  <si>
+    <t>p-Methylcatechol</t>
+  </si>
+  <si>
+    <t>O=Cc1ccccc1C=O</t>
+  </si>
+  <si>
+    <t>643-79-8</t>
+  </si>
+  <si>
+    <t>ortho-Phthalaldehyde</t>
+  </si>
+  <si>
+    <t>CCCOC(=O)c1ccc(O)cc1</t>
+  </si>
+  <si>
+    <t>94-13-3</t>
+  </si>
+  <si>
+    <t>Propyl-4-hydroxybenzoate</t>
+  </si>
+  <si>
+    <t>Oc1ccc(/C=C/c2cc(O)cc(O)c2)cc1</t>
+  </si>
+  <si>
+    <t>501-36-0</t>
+  </si>
+  <si>
+    <t>Resveratrol</t>
+  </si>
+  <si>
+    <t>CC(CCC(=O)O)(c1ccc(O)cc1)c1ccc(O)cc1</t>
+  </si>
+  <si>
+    <t>126-00-1</t>
+  </si>
+  <si>
+    <t>Diphenolic acid</t>
+  </si>
+  <si>
+    <t>OCCOc1ccccc1</t>
+  </si>
+  <si>
+    <t>122-99-6</t>
+  </si>
+  <si>
+    <t>Ethylene glycol monophenyl ether</t>
+  </si>
+  <si>
+    <t>Cc1cccc(C(=O)O)c1</t>
+  </si>
+  <si>
+    <t>99-04-7</t>
+  </si>
+  <si>
+    <t>m-Toluic acid</t>
+  </si>
+  <si>
+    <t>CCCCOC(=O)c1ccc(O)cc1</t>
+  </si>
+  <si>
+    <t>94-26-8</t>
+  </si>
+  <si>
+    <t>Butyl Paraben</t>
+  </si>
+  <si>
+    <t>Cc1ccc(O)cc1C</t>
+  </si>
+  <si>
+    <t>95-65-8</t>
+  </si>
+  <si>
+    <t>3,4-Dimethyl phenol</t>
+  </si>
+  <si>
+    <t>Cc1cccc2ccccc12</t>
+  </si>
+  <si>
+    <t>1321-94-4</t>
+  </si>
+  <si>
+    <t>Methyl naphthalene</t>
+  </si>
+  <si>
+    <t>Cc1ccc(C)c(O)c1</t>
+  </si>
+  <si>
+    <t>95-87-4</t>
+  </si>
+  <si>
+    <t>2,5-Dimethyl phenol</t>
+  </si>
+  <si>
+    <t>Cc1ccc(O)c(C)c1</t>
+  </si>
+  <si>
+    <t>105-67-9</t>
+  </si>
+  <si>
+    <t>2,4-Dimethylphenol</t>
+  </si>
+  <si>
+    <t>CC(C)OC(=O)Cc1ccccc1</t>
+  </si>
+  <si>
+    <t>4861-85-2</t>
+  </si>
+  <si>
+    <t>Isopropyl phenylacetate</t>
+  </si>
+  <si>
+    <t>C=CCc1cc(OC)c2c(c1)OCO2</t>
+  </si>
+  <si>
+    <t>607-91-0</t>
+  </si>
+  <si>
+    <t>Myristicin</t>
+  </si>
+  <si>
+    <t>O=C(O)/C=C/c1ccc(/C=C/C(=O)O)cc1</t>
+  </si>
+  <si>
+    <t>16323-43-6</t>
+  </si>
+  <si>
+    <t>3,3'-(1,4-Phenylene)bis-2-propenoic acid</t>
+  </si>
+  <si>
+    <t>CC(O)COc1ccccc1</t>
+  </si>
+  <si>
+    <t>770-35-4</t>
+  </si>
+  <si>
+    <t>Propylene glycol phenyl ether</t>
+  </si>
+  <si>
+    <t>CCCCCCOC(=O)c1ccccc1</t>
+  </si>
+  <si>
+    <t>6789-88-4</t>
+  </si>
+  <si>
+    <t>Hexylbenzoate</t>
+  </si>
+  <si>
+    <t>Cc1c(O)cccc1O</t>
+  </si>
+  <si>
+    <t>608-25-3</t>
+  </si>
+  <si>
+    <t>2-Methyl-1,3-benzenediol</t>
+  </si>
+  <si>
+    <t>Cc1ccc2ccccc2c1</t>
+  </si>
+  <si>
+    <t>91-57-6</t>
+  </si>
+  <si>
+    <t>2-Methylnaphthalene</t>
+  </si>
+  <si>
+    <t>CC(=O)OC(C(=O)c1ccccc1)c1ccccc1</t>
+  </si>
+  <si>
+    <t>574-06-1</t>
+  </si>
+  <si>
+    <t>Benzoin acetate</t>
+  </si>
+  <si>
+    <t>C=Cc1cccc(C)c1</t>
+  </si>
+  <si>
+    <t>25013-15-4</t>
+  </si>
+  <si>
+    <t>Vinyl toluene</t>
+  </si>
+  <si>
+    <t>Cc1ccc2cc3c(ccc4ccccc43)c3c2c1CC3</t>
+  </si>
+  <si>
+    <t>56-49-5</t>
+  </si>
+  <si>
+    <t>3-Methylcholanthrene</t>
+  </si>
+  <si>
+    <t>O=c1cc(-c2ccccc2)oc2ccc3ccccc3c12</t>
+  </si>
+  <si>
+    <t>6051-87-2</t>
+  </si>
+  <si>
+    <t>5,6-Benzoflavone</t>
+  </si>
+  <si>
+    <t>O=c1c(-c2ccc(O)cc2)coc2cc(O)cc(O)c12</t>
+  </si>
+  <si>
+    <t>446-72-0</t>
+  </si>
+  <si>
+    <t>Genistein</t>
+  </si>
+  <si>
+    <t>Cc1ccc2oc(=O)ccc2c1</t>
+  </si>
+  <si>
+    <t>92-48-8</t>
+  </si>
+  <si>
+    <t>Methyl coumarin</t>
   </si>
 </sst>
 </file>
@@ -5434,7 +5812,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F556"/>
+  <dimension ref="A1:F598"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
@@ -5442,7 +5820,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -16565,6 +16945,846 @@
         <v>0</v>
       </c>
     </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B557">
+        <v>0.17</v>
+      </c>
+      <c r="C557">
+        <v>0</v>
+      </c>
+      <c r="D557" t="s">
+        <v>1672</v>
+      </c>
+      <c r="E557" t="s">
+        <v>1673</v>
+      </c>
+      <c r="F557">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B558">
+        <v>-0.05</v>
+      </c>
+      <c r="C558">
+        <v>0</v>
+      </c>
+      <c r="D558" t="s">
+        <v>1675</v>
+      </c>
+      <c r="E558" t="s">
+        <v>1676</v>
+      </c>
+      <c r="F558">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A559" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B559">
+        <v>0.06</v>
+      </c>
+      <c r="C559">
+        <v>0</v>
+      </c>
+      <c r="D559" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E559" t="s">
+        <v>1679</v>
+      </c>
+      <c r="F559">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B560">
+        <v>0.16</v>
+      </c>
+      <c r="C560">
+        <v>0</v>
+      </c>
+      <c r="D560" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E560" t="s">
+        <v>1682</v>
+      </c>
+      <c r="F560">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="561" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B561">
+        <v>0.08</v>
+      </c>
+      <c r="C561">
+        <v>0</v>
+      </c>
+      <c r="D561" t="s">
+        <v>1684</v>
+      </c>
+      <c r="E561" t="s">
+        <v>1685</v>
+      </c>
+      <c r="F561">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B562">
+        <v>0.34</v>
+      </c>
+      <c r="C562">
+        <v>0</v>
+      </c>
+      <c r="D562" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E562" t="s">
+        <v>1688</v>
+      </c>
+      <c r="F562">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B563">
+        <v>0.26</v>
+      </c>
+      <c r="C563">
+        <v>0</v>
+      </c>
+      <c r="D563" t="s">
+        <v>1690</v>
+      </c>
+      <c r="E563" t="s">
+        <v>1691</v>
+      </c>
+      <c r="F563">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A564" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B564">
+        <v>0.04</v>
+      </c>
+      <c r="C564">
+        <v>0</v>
+      </c>
+      <c r="D564" t="s">
+        <v>1693</v>
+      </c>
+      <c r="E564" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F564">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B565">
+        <v>0.12</v>
+      </c>
+      <c r="C565">
+        <v>0</v>
+      </c>
+      <c r="D565" t="s">
+        <v>1696</v>
+      </c>
+      <c r="E565" t="s">
+        <v>1697</v>
+      </c>
+      <c r="F565">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="566" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B566">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C566">
+        <v>0</v>
+      </c>
+      <c r="D566" t="s">
+        <v>1699</v>
+      </c>
+      <c r="E566" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F566">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="567" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>1701</v>
+      </c>
+      <c r="B567">
+        <v>0.01</v>
+      </c>
+      <c r="C567">
+        <v>0</v>
+      </c>
+      <c r="D567" t="s">
+        <v>1702</v>
+      </c>
+      <c r="E567" t="s">
+        <v>1703</v>
+      </c>
+      <c r="F567">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="568" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B568">
+        <v>0.16</v>
+      </c>
+      <c r="C568">
+        <v>0</v>
+      </c>
+      <c r="D568" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E568" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F568">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="569" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B569">
+        <v>0.41</v>
+      </c>
+      <c r="C569">
+        <v>0</v>
+      </c>
+      <c r="D569" t="s">
+        <v>1708</v>
+      </c>
+      <c r="E569" t="s">
+        <v>1709</v>
+      </c>
+      <c r="F569">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="570" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B570">
+        <v>0.04</v>
+      </c>
+      <c r="C570">
+        <v>0</v>
+      </c>
+      <c r="D570" t="s">
+        <v>1711</v>
+      </c>
+      <c r="E570" t="s">
+        <v>1712</v>
+      </c>
+      <c r="F570">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="571" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B571">
+        <v>0.36</v>
+      </c>
+      <c r="C571">
+        <v>1</v>
+      </c>
+      <c r="D571" t="s">
+        <v>1714</v>
+      </c>
+      <c r="E571" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F571">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="572" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B572">
+        <v>0.15</v>
+      </c>
+      <c r="C572">
+        <v>1</v>
+      </c>
+      <c r="D572" t="s">
+        <v>1717</v>
+      </c>
+      <c r="E572" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F572">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="573" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B573">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C573">
+        <v>0</v>
+      </c>
+      <c r="D573" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E573" t="s">
+        <v>1721</v>
+      </c>
+      <c r="F573">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="574" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B574">
+        <v>0.41</v>
+      </c>
+      <c r="C574">
+        <v>0</v>
+      </c>
+      <c r="D574" t="s">
+        <v>1723</v>
+      </c>
+      <c r="E574" t="s">
+        <v>1724</v>
+      </c>
+      <c r="F574">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="575" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B575">
+        <v>0.16</v>
+      </c>
+      <c r="C575">
+        <v>1</v>
+      </c>
+      <c r="D575" t="s">
+        <v>1726</v>
+      </c>
+      <c r="E575" t="s">
+        <v>1727</v>
+      </c>
+      <c r="F575">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="576" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B576">
+        <v>0.05</v>
+      </c>
+      <c r="C576">
+        <v>0</v>
+      </c>
+      <c r="D576" t="s">
+        <v>1729</v>
+      </c>
+      <c r="E576" t="s">
+        <v>1730</v>
+      </c>
+      <c r="F576">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="577" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B577">
+        <v>0.83</v>
+      </c>
+      <c r="C577">
+        <v>0</v>
+      </c>
+      <c r="D577" t="s">
+        <v>1732</v>
+      </c>
+      <c r="E577" t="s">
+        <v>1733</v>
+      </c>
+      <c r="F577">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="578" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B578">
+        <v>-0.18</v>
+      </c>
+      <c r="C578">
+        <v>0</v>
+      </c>
+      <c r="D578" t="s">
+        <v>1735</v>
+      </c>
+      <c r="E578" t="s">
+        <v>1736</v>
+      </c>
+      <c r="F578">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="579" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B579">
+        <v>0.08</v>
+      </c>
+      <c r="C579">
+        <v>0</v>
+      </c>
+      <c r="D579" t="s">
+        <v>1738</v>
+      </c>
+      <c r="E579" t="s">
+        <v>1739</v>
+      </c>
+      <c r="F579">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="580" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B580">
+        <v>0.06</v>
+      </c>
+      <c r="C580">
+        <v>0</v>
+      </c>
+      <c r="D580" t="s">
+        <v>1741</v>
+      </c>
+      <c r="E580" t="s">
+        <v>1742</v>
+      </c>
+      <c r="F580">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="581" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B581">
+        <v>-0.05</v>
+      </c>
+      <c r="C581">
+        <v>0</v>
+      </c>
+      <c r="D581" t="s">
+        <v>1744</v>
+      </c>
+      <c r="E581" t="s">
+        <v>1745</v>
+      </c>
+      <c r="F581">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="582" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A582" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B582">
+        <v>0.31</v>
+      </c>
+      <c r="C582">
+        <v>0</v>
+      </c>
+      <c r="D582" t="s">
+        <v>1747</v>
+      </c>
+      <c r="E582" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F582">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="583" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A583" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B583">
+        <v>-0.02</v>
+      </c>
+      <c r="C583">
+        <v>0</v>
+      </c>
+      <c r="D583" t="s">
+        <v>1750</v>
+      </c>
+      <c r="E583" t="s">
+        <v>1751</v>
+      </c>
+      <c r="F583">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="584" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A584" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B584">
+        <v>0.25</v>
+      </c>
+      <c r="C584">
+        <v>0</v>
+      </c>
+      <c r="D584" t="s">
+        <v>1753</v>
+      </c>
+      <c r="E584" t="s">
+        <v>1754</v>
+      </c>
+      <c r="F584">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="585" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A585" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B585">
+        <v>0.47</v>
+      </c>
+      <c r="C585">
+        <v>1</v>
+      </c>
+      <c r="D585" t="s">
+        <v>1756</v>
+      </c>
+      <c r="E585" t="s">
+        <v>1757</v>
+      </c>
+      <c r="F585">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="586" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A586" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B586">
+        <v>0.03</v>
+      </c>
+      <c r="C586">
+        <v>0</v>
+      </c>
+      <c r="D586" t="s">
+        <v>1759</v>
+      </c>
+      <c r="E586" t="s">
+        <v>1760</v>
+      </c>
+      <c r="F586">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="587" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A587" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B587">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C587">
+        <v>0</v>
+      </c>
+      <c r="D587" t="s">
+        <v>1762</v>
+      </c>
+      <c r="E587" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F587">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="588" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A588" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B588">
+        <v>0.41</v>
+      </c>
+      <c r="C588">
+        <v>0</v>
+      </c>
+      <c r="D588" t="s">
+        <v>1765</v>
+      </c>
+      <c r="E588" t="s">
+        <v>1766</v>
+      </c>
+      <c r="F588">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="589" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A589" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B589">
+        <v>0.21</v>
+      </c>
+      <c r="C589">
+        <v>0</v>
+      </c>
+      <c r="D589" t="s">
+        <v>1768</v>
+      </c>
+      <c r="E589" t="s">
+        <v>1769</v>
+      </c>
+      <c r="F589">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="590" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A590" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B590">
+        <v>-0.03</v>
+      </c>
+      <c r="C590">
+        <v>0</v>
+      </c>
+      <c r="D590" t="s">
+        <v>1771</v>
+      </c>
+      <c r="E590" t="s">
+        <v>1772</v>
+      </c>
+      <c r="F590">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="591" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A591" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B591">
+        <v>0.16</v>
+      </c>
+      <c r="C591">
+        <v>0</v>
+      </c>
+      <c r="D591" t="s">
+        <v>1774</v>
+      </c>
+      <c r="E591" t="s">
+        <v>1775</v>
+      </c>
+      <c r="F591">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="592" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A592" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B592">
+        <v>0.04</v>
+      </c>
+      <c r="C592">
+        <v>0</v>
+      </c>
+      <c r="D592" t="s">
+        <v>1777</v>
+      </c>
+      <c r="E592" t="s">
+        <v>1778</v>
+      </c>
+      <c r="F592">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="593" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A593" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B593">
+        <v>0.2</v>
+      </c>
+      <c r="C593">
+        <v>0</v>
+      </c>
+      <c r="D593" t="s">
+        <v>1780</v>
+      </c>
+      <c r="E593" t="s">
+        <v>1781</v>
+      </c>
+      <c r="F593">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="594" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A594" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B594">
+        <v>0.01</v>
+      </c>
+      <c r="C594">
+        <v>0</v>
+      </c>
+      <c r="D594" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E594" t="s">
+        <v>1784</v>
+      </c>
+      <c r="F594">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="595" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A595" t="s">
+        <v>1785</v>
+      </c>
+      <c r="B595">
+        <v>0.91</v>
+      </c>
+      <c r="C595">
+        <v>1</v>
+      </c>
+      <c r="D595" t="s">
+        <v>1786</v>
+      </c>
+      <c r="E595" t="s">
+        <v>1787</v>
+      </c>
+      <c r="F595">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="596" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B596">
+        <v>0.13</v>
+      </c>
+      <c r="C596">
+        <v>0</v>
+      </c>
+      <c r="D596" t="s">
+        <v>1789</v>
+      </c>
+      <c r="E596" t="s">
+        <v>1790</v>
+      </c>
+      <c r="F596">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="597" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A597" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B597">
+        <v>0.17</v>
+      </c>
+      <c r="C597">
+        <v>1</v>
+      </c>
+      <c r="D597" t="s">
+        <v>1792</v>
+      </c>
+      <c r="E597" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F597">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="598" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A598" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B598">
+        <v>0.38</v>
+      </c>
+      <c r="C598">
+        <v>0</v>
+      </c>
+      <c r="D598" t="s">
+        <v>1795</v>
+      </c>
+      <c r="E598" t="s">
+        <v>1796</v>
+      </c>
+      <c r="F598">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>